<commit_message>
Updated app.py and added new files
</commit_message>
<xml_diff>
--- a/uploads/participants_data.xlsx
+++ b/uploads/participants_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\princ\OneDrive\Desktop\E_CERTIFICATE\certificate_proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\princ\OneDrive\Desktop\certificate_proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FC286E-95AB-4D53-BB0E-B40785F555D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA95D9E6-7B9D-4BA0-917A-ACA8EFE9641A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{74C0C3D2-99F0-4FAB-9F4A-C50C53D5816D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>prince960876@gmail.com</t>
   </si>
@@ -66,19 +66,13 @@
     <t>Backend Development</t>
   </si>
   <si>
-    <t>Priyanshi mandloi</t>
-  </si>
-  <si>
-    <t>priyanshimandloi06@gmail.com</t>
-  </si>
-  <si>
     <t>Designer</t>
   </si>
   <si>
-    <t>Asmi</t>
-  </si>
-  <si>
-    <t>asmich1906@gmail.com</t>
+    <t>Pawan kushwaha</t>
+  </si>
+  <si>
+    <t>pawankushwaha91719171@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -510,7 +504,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,13 +564,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D4" s="6">
         <v>45844</v>
@@ -584,26 +578,17 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="6">
-        <v>45844</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{9C7848AF-C041-48D1-BDC2-C916FFB25649}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{C00A926D-B1FF-4D31-8020-28A2749BC0E8}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{882DC290-0CE5-4267-B58F-2E67CC02D875}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{ACA45DB4-F253-472B-8FB8-52AAA0FD4786}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{2B0D2077-4ED0-486D-BAE7-AC6AEB088BB0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>